<commit_message>
MML-23: Test cambio de base segun datasets disponibles para todas las regiones
</commit_message>
<xml_diff>
--- a/notebooks/data/DP_LIVE_03012023234123498.xlsx
+++ b/notebooks/data/DP_LIVE_03012023234123498.xlsx
@@ -1,12 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26129"/>
   <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_946CFD94455DE3A4B48695F6D8038024668A0D66" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="DP_LIVE_03012023234123498" sheetId="1" r:id="rId4"/>
+    <sheet name="DP_LIVE_03012023234123498" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -244,15 +248,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -263,39 +268,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -485,20 +495,23 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -541,13 +554,13 @@
         <v>12</v>
       </c>
       <c r="F2" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G2" s="2">
-        <v>1477553.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1477553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -564,13 +577,13 @@
         <v>12</v>
       </c>
       <c r="F3" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G3" s="2">
-        <v>775009.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>775009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -587,13 +600,13 @@
         <v>12</v>
       </c>
       <c r="F4" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G4" s="2">
-        <v>775634.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>775634</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -610,13 +623,13 @@
         <v>12</v>
       </c>
       <c r="F5" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G5" s="2">
-        <v>1212304.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>1212304</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -633,13 +646,13 @@
         <v>12</v>
       </c>
       <c r="F6" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G6" s="2">
-        <v>1.2424986E7</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>12424986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -656,13 +669,13 @@
         <v>12</v>
       </c>
       <c r="F7" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G7" s="2">
-        <v>6871679.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>6871679</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -679,13 +692,13 @@
         <v>12</v>
       </c>
       <c r="F8" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G8" s="2">
-        <v>863657.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>863657</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -702,13 +715,13 @@
         <v>12</v>
       </c>
       <c r="F9" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G9" s="2">
-        <v>770109.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>770109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -725,13 +738,13 @@
         <v>12</v>
       </c>
       <c r="F10" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G10" s="2">
-        <v>744783.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>744783</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -748,13 +761,13 @@
         <v>12</v>
       </c>
       <c r="F11" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G11" s="2">
-        <v>575041.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>575041</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -771,13 +784,13 @@
         <v>12</v>
       </c>
       <c r="F12" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G12" s="2">
-        <v>1.36036522E8</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>136036522</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -794,13 +807,13 @@
         <v>12</v>
       </c>
       <c r="F13" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G13" s="2">
-        <v>1.38277175E8</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>138277175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -817,13 +830,13 @@
         <v>12</v>
       </c>
       <c r="F14" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G14" s="2">
-        <v>794405.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>794405</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
@@ -840,13 +853,13 @@
         <v>12</v>
       </c>
       <c r="F15" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G15" s="2">
-        <v>689895.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>689895</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -863,13 +876,13 @@
         <v>12</v>
       </c>
       <c r="F16" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G16" s="2">
-        <v>1.05101901E8</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>105101901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -886,13 +899,13 @@
         <v>12</v>
       </c>
       <c r="F17" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G17" s="2">
-        <v>8.72624771E8</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>872624771</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -909,13 +922,13 @@
         <v>12</v>
       </c>
       <c r="F18" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G18" s="2">
-        <v>84831.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>84831</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1" t="s">
         <v>29</v>
       </c>
@@ -932,13 +945,13 @@
         <v>12</v>
       </c>
       <c r="F19" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G19" s="2">
-        <v>8913552.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>8913552</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
@@ -955,13 +968,13 @@
         <v>12</v>
       </c>
       <c r="F20" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G20" s="2">
-        <v>78215.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>78215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -978,13 +991,13 @@
         <v>12</v>
       </c>
       <c r="F21" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G21" s="2">
-        <v>1430959.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>1430959</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -1001,13 +1014,13 @@
         <v>12</v>
       </c>
       <c r="F22" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G22" s="2">
-        <v>974983.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>974983</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1024,13 +1037,13 @@
         <v>12</v>
       </c>
       <c r="F23" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G23" s="2">
-        <v>1742879.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>1742879</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1047,13 +1060,13 @@
         <v>12</v>
       </c>
       <c r="F24" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G24" s="2">
-        <v>575688.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>575688</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1070,13 +1083,13 @@
         <v>12</v>
       </c>
       <c r="F25" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G25" s="2">
-        <v>516433.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>516433</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1093,13 +1106,13 @@
         <v>12</v>
       </c>
       <c r="F26" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G26" s="2">
-        <v>630839.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>630839</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -1116,13 +1129,13 @@
         <v>12</v>
       </c>
       <c r="F27" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G27" s="2">
-        <v>8852247.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>8852247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1" t="s">
         <v>38</v>
       </c>
@@ -1139,13 +1152,13 @@
         <v>12</v>
       </c>
       <c r="F28" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G28" s="2">
-        <v>1187726.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>1187726</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
@@ -1162,13 +1175,13 @@
         <v>12</v>
       </c>
       <c r="F29" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G29" s="2">
-        <v>138398.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>138398</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1" t="s">
         <v>40</v>
       </c>
@@ -1185,13 +1198,13 @@
         <v>12</v>
       </c>
       <c r="F30" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G30" s="2">
-        <v>684601.0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>684601</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>
@@ -1208,13 +1221,13 @@
         <v>12</v>
       </c>
       <c r="F31" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G31" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -1231,13 +1244,13 @@
         <v>12</v>
       </c>
       <c r="F32" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G32" s="2">
-        <v>2181557.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>2181557</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1" t="s">
         <v>43</v>
       </c>
@@ -1254,13 +1267,13 @@
         <v>12</v>
       </c>
       <c r="F33" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G33" s="2">
-        <v>3.97689401E8</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>397689401</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1" t="s">
         <v>44</v>
       </c>
@@ -1277,13 +1290,13 @@
         <v>12</v>
       </c>
       <c r="F34" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G34" s="2">
-        <v>4183811.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>4183811</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
@@ -1300,13 +1313,13 @@
         <v>12</v>
       </c>
       <c r="F35" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G35" s="2">
-        <v>1.328016627E9</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>1328016627</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1" t="s">
         <v>46</v>
       </c>
@@ -1323,13 +1336,13 @@
         <v>12</v>
       </c>
       <c r="F36" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G36" s="2">
-        <v>534908.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>534908</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1" t="s">
         <v>47</v>
       </c>
@@ -1346,13 +1359,13 @@
         <v>12</v>
       </c>
       <c r="F37" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G37" s="2">
-        <v>2.0647793E7</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>20647793</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1" t="s">
         <v>48</v>
       </c>
@@ -1369,13 +1382,13 @@
         <v>12</v>
       </c>
       <c r="F38" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G38" s="2">
-        <v>4.695658691E9</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>4695658691</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
@@ -1392,13 +1405,13 @@
         <v>12</v>
       </c>
       <c r="F39" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G39" s="2">
-        <v>3751633.0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>3751633</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1" t="s">
         <v>50</v>
       </c>
@@ -1415,13 +1428,13 @@
         <v>12</v>
       </c>
       <c r="F40" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G40" s="2">
-        <v>2.4124181E7</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>24124181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1" t="s">
         <v>51</v>
       </c>
@@ -1438,13 +1451,13 @@
         <v>12</v>
       </c>
       <c r="F41" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G41" s="2">
-        <v>570149.0</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>570149</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1" t="s">
         <v>52</v>
       </c>
@@ -1461,13 +1474,13 @@
         <v>12</v>
       </c>
       <c r="F42" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G42" s="2">
-        <v>6426701.0</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>6426701</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1" t="s">
         <v>53</v>
       </c>
@@ -1484,13 +1497,13 @@
         <v>12</v>
       </c>
       <c r="F43" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G43" s="2">
-        <v>484537.0</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>484537</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
         <v>54</v>
       </c>
@@ -1507,13 +1520,13 @@
         <v>12</v>
       </c>
       <c r="F44" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G44" s="2">
-        <v>44272.0</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>44272</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1" t="s">
         <v>55</v>
       </c>
@@ -1530,13 +1543,13 @@
         <v>12</v>
       </c>
       <c r="F45" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G45" s="2">
-        <v>1649027.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>1649027</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="1" t="s">
         <v>56</v>
       </c>
@@ -1553,13 +1566,13 @@
         <v>12</v>
       </c>
       <c r="F46" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G46" s="2">
-        <v>721081.0</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>721081</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1" t="s">
         <v>57</v>
       </c>
@@ -1576,13 +1589,13 @@
         <v>12</v>
       </c>
       <c r="F47" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G47" s="2">
-        <v>1.0256822E7</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>10256822</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
         <v>58</v>
       </c>
@@ -1599,13 +1612,13 @@
         <v>12</v>
       </c>
       <c r="F48" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G48" s="2">
-        <v>3.40991882E8</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>340991882</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
         <v>59</v>
       </c>
@@ -1622,13 +1635,13 @@
         <v>12</v>
       </c>
       <c r="F49" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G49" s="2">
-        <v>676282.0</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>676282</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
         <v>60</v>
       </c>
@@ -1645,13 +1658,13 @@
         <v>12</v>
       </c>
       <c r="F50" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G50" s="2">
-        <v>3324668.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>3324668</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1" t="s">
         <v>61</v>
       </c>
@@ -1668,13 +1681,13 @@
         <v>12</v>
       </c>
       <c r="F51" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G51" s="2">
-        <v>615185.0</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>615185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1" t="s">
         <v>62</v>
       </c>
@@ -1691,13 +1704,13 @@
         <v>12</v>
       </c>
       <c r="F52" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G52" s="2">
-        <v>586426.0</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>586426</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
@@ -1714,13 +1727,13 @@
         <v>12</v>
       </c>
       <c r="F53" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G53" s="2">
-        <v>1613577.0</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>1613577</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="1" t="s">
         <v>64</v>
       </c>
@@ -1737,13 +1750,13 @@
         <v>12</v>
       </c>
       <c r="F54" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G54" s="2">
-        <v>1.8970187E7</v>
-      </c>
-    </row>
-    <row r="55">
+        <v>18970187</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="1" t="s">
         <v>65</v>
       </c>
@@ -1760,13 +1773,13 @@
         <v>12</v>
       </c>
       <c r="F55" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G55" s="2">
-        <v>419258.0</v>
-      </c>
-    </row>
-    <row r="56">
+        <v>419258</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="1" t="s">
         <v>66</v>
       </c>
@@ -1783,13 +1796,13 @@
         <v>12</v>
       </c>
       <c r="F56" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G56" s="2">
-        <v>6011433.0</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>6011433</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1" t="s">
         <v>67</v>
       </c>
@@ -1806,13 +1819,13 @@
         <v>12</v>
       </c>
       <c r="F57" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G57" s="2">
-        <v>1.013434631E9</v>
-      </c>
-    </row>
-    <row r="58">
+        <v>1013434631</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="1" t="s">
         <v>68</v>
       </c>
@@ -1829,13 +1842,13 @@
         <v>12</v>
       </c>
       <c r="F58" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G58" s="2">
-        <v>402344.0</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>402344</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="1" t="s">
         <v>69</v>
       </c>
@@ -1852,13 +1865,13 @@
         <v>12</v>
       </c>
       <c r="F59" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G59" s="2">
-        <v>88598.0</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>88598</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="1" t="s">
         <v>70</v>
       </c>
@@ -1875,13 +1888,13 @@
         <v>12</v>
       </c>
       <c r="F60" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G60" s="2">
-        <v>686815.0</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>686815</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="1" t="s">
         <v>71</v>
       </c>
@@ -1898,13 +1911,13 @@
         <v>12</v>
       </c>
       <c r="F61" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G61" s="2">
-        <v>4.2255635E7</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>42255635</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1" t="s">
         <v>72</v>
       </c>
@@ -1921,13 +1934,13 @@
         <v>12</v>
       </c>
       <c r="F62" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G62" s="2">
-        <v>4.0821015E7</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>40821015</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1" t="s">
         <v>73</v>
       </c>
@@ -1944,13 +1957,13 @@
         <v>12</v>
       </c>
       <c r="F63" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G63" s="2">
-        <v>804572.0</v>
-      </c>
-    </row>
-    <row r="64">
+        <v>804572</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1" t="s">
         <v>74</v>
       </c>
@@ -1967,13 +1980,13 @@
         <v>12</v>
       </c>
       <c r="F64" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G64" s="2">
-        <v>2.32801392E8</v>
-      </c>
-    </row>
-    <row r="65">
+        <v>232801392</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="1" t="s">
         <v>75</v>
       </c>
@@ -1990,13 +2003,13 @@
         <v>12</v>
       </c>
       <c r="F65" s="1">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="G65" s="2">
-        <v>2.46786667E8</v>
+        <v>246786667</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
</xml_diff>